<commit_message>
adding updated Excel files
</commit_message>
<xml_diff>
--- a/Figure1.xlsx
+++ b/Figure1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walid/Desktop/DI/Research/Telegram-2025/New Media Society/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walid/Desktop/DI/Research/Telegram-2025/Contingencies &amp; Crisis Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BCB15C-C1DC-3544-8FEB-25A24FF14AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A243E52-5582-C641-819C-EFA1D5ABC865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="3320" windowWidth="26040" windowHeight="14920" xr2:uid="{A0D85137-C6A8-7E48-A0F4-4B68D6F78C71}"/>
+    <workbookView xWindow="0" yWindow="3320" windowWidth="29140" windowHeight="14920" xr2:uid="{A0D85137-C6A8-7E48-A0F4-4B68D6F78C71}"/>
   </bookViews>
   <sheets>
     <sheet name="figure1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Kanal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>u_now</t>
   </si>
@@ -71,62 +68,41 @@
     <t>xydessa</t>
   </si>
   <si>
-    <t>bozhejakekonchene</t>
-  </si>
-  <si>
     <t>legitimniy</t>
   </si>
   <si>
     <t>asupersharij</t>
   </si>
   <si>
-    <t>v_zelenskiy_official</t>
-  </si>
-  <si>
     <t>muzyka_xmusix</t>
   </si>
   <si>
-    <t>Nov</t>
+    <t>Month</t>
   </si>
   <si>
-    <t>Dec</t>
+    <t>bozhejake-
+konchene</t>
   </si>
   <si>
-    <t>Jan</t>
+    <t>v_zelenskiy
+_official</t>
   </si>
   <si>
-    <t>Feb</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Jul</t>
-  </si>
-  <si>
-    <t>Aug</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>Oct</t>
+    <t>Subtotal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,6 +116,20 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -175,17 +165,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -241,45 +244,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -337,13 +344,13 @@
             <c:v>uniannet</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="sq">
+            <a:ln w="28575" cap="flat">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:prstDash val="dash"/>
               <a:bevel/>
-              <a:headEnd type="diamond"/>
+              <a:headEnd type="none"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -351,45 +358,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -459,45 +470,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -567,45 +582,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -663,10 +682,11 @@
             <c:v>voynareal</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="28575" cap="rnd" cmpd="dbl">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -675,45 +695,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -783,45 +807,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -885,6 +913,7 @@
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -893,45 +922,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -989,7 +1022,7 @@
             <c:v>lachentyt</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="44450" cap="rnd" cmpd="thinThick">
               <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
@@ -1003,45 +1036,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1093,12 +1130,13 @@
             <c:v>ukrainenow</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="28575" cap="sq" cmpd="tri">
               <a:solidFill>
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="lgDashDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1107,45 +1145,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1217,45 +1259,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1327,45 +1373,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1437,45 +1487,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1548,45 +1602,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1659,45 +1717,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1770,45 +1832,49 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="12"/>
-              <c:pt idx="0">
-                <c:v>Nov</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>Dec</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>Jan</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>Feb</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>Mar</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>Apr</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>May</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>Jun</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>Jul</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>Aug</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>Sep</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>Oct</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:numRef>
+              <c:f>figure1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44835</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numLit>
@@ -1878,7 +1944,115 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Month</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> when the posts were published</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.35337760950290725"/>
+              <c:y val="0.78473917322834641"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-QA"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1900,7 +2074,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1917,7 +2091,7 @@
         </c:txPr>
         <c:crossAx val="137195136"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
@@ -1926,6 +2100,8 @@
         <c:axId val="137195136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="15000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1943,7 +2119,130 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of posts </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>(N=341,680)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.247027741083224E-3"/>
+              <c:y val="0.27624568480664052"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-QA"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1959,7 +2258,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1976,7 +2275,7 @@
         </c:txPr>
         <c:crossAx val="14127344"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1992,17 +2291,22 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.3341289655866185E-2"/>
-          <c:y val="0.87056254240764996"/>
-          <c:w val="0.88217628284269345"/>
-          <c:h val="0.1162217348081991"/>
+          <c:x val="2.4612476964315629E-2"/>
+          <c:y val="0.85394172408136482"/>
+          <c:w val="0.95844755104764445"/>
+          <c:h val="0.1360215715223097"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -2011,12 +2315,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2631,15 +2932,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2986,663 +3287,757 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B005979C-BA19-6B46-A813-5276345883D6}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="16" max="16" width="17" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B2" s="2">
+        <v>589</v>
+      </c>
+      <c r="C2" s="2">
+        <v>539</v>
+      </c>
+      <c r="D2" s="2">
+        <v>867</v>
+      </c>
+      <c r="E2" s="2">
+        <v>805</v>
+      </c>
+      <c r="F2" s="2">
+        <v>328</v>
+      </c>
+      <c r="G2" s="2">
+        <v>764</v>
+      </c>
+      <c r="H2" s="2">
+        <v>581</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>95</v>
+      </c>
+      <c r="K2" s="2">
+        <v>590</v>
+      </c>
+      <c r="L2" s="2">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2">
+        <v>271</v>
+      </c>
+      <c r="N2" s="2">
+        <v>185</v>
+      </c>
+      <c r="O2" s="2">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B3" s="2">
+        <v>549</v>
+      </c>
+      <c r="C3" s="2">
+        <v>525</v>
+      </c>
+      <c r="D3" s="2">
+        <v>694</v>
+      </c>
+      <c r="E3" s="2">
+        <v>815</v>
+      </c>
+      <c r="F3" s="2">
+        <v>319</v>
+      </c>
+      <c r="G3" s="2">
+        <v>768</v>
+      </c>
+      <c r="H3" s="2">
+        <v>500</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>74</v>
+      </c>
+      <c r="K3" s="2">
+        <v>633</v>
+      </c>
+      <c r="L3" s="2">
+        <v>23</v>
+      </c>
+      <c r="M3" s="2">
+        <v>189</v>
+      </c>
+      <c r="N3" s="2">
+        <v>213</v>
+      </c>
+      <c r="O3" s="2">
+        <v>7</v>
+      </c>
+      <c r="P3" s="2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B4" s="2">
+        <v>682</v>
+      </c>
+      <c r="C4" s="2">
+        <v>856</v>
+      </c>
+      <c r="D4" s="2">
+        <v>734</v>
+      </c>
+      <c r="E4" s="2">
+        <v>772</v>
+      </c>
+      <c r="F4" s="2">
+        <v>489</v>
+      </c>
+      <c r="G4" s="2">
+        <v>538</v>
+      </c>
+      <c r="H4" s="2">
+        <v>492</v>
+      </c>
+      <c r="I4" s="2">
+        <v>477</v>
+      </c>
+      <c r="J4" s="2">
+        <v>92</v>
+      </c>
+      <c r="K4" s="2">
+        <v>642</v>
+      </c>
+      <c r="L4" s="2">
+        <v>9</v>
+      </c>
+      <c r="M4" s="2">
+        <v>232</v>
+      </c>
+      <c r="N4" s="2">
+        <v>218</v>
+      </c>
+      <c r="O4" s="2">
+        <v>39</v>
+      </c>
+      <c r="P4" s="2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4434</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3635</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3799</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1505</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3464</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2864</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3344</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2655</v>
+      </c>
+      <c r="J5" s="2">
+        <v>737</v>
+      </c>
+      <c r="K5" s="2">
+        <v>522</v>
+      </c>
+      <c r="L5" s="2">
+        <v>27</v>
+      </c>
+      <c r="M5" s="2">
+        <v>855</v>
+      </c>
+      <c r="N5" s="2">
+        <v>279</v>
+      </c>
+      <c r="O5" s="2">
+        <v>117</v>
+      </c>
+      <c r="P5" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B6" s="2">
+        <v>14760</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9280</v>
+      </c>
+      <c r="D6" s="2">
+        <v>11055</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4296</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5808</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5380</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4938</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3645</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4760</v>
+      </c>
+      <c r="K6" s="2">
+        <v>499</v>
+      </c>
+      <c r="L6" s="2">
+        <v>964</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1145</v>
+      </c>
+      <c r="N6" s="2">
+        <v>323</v>
+      </c>
+      <c r="O6" s="2">
+        <v>291</v>
+      </c>
+      <c r="P6" s="2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10085</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7736</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6215</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3788</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3187</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2914</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2745</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2865</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2813</v>
+      </c>
+      <c r="K7" s="2">
+        <v>569</v>
+      </c>
+      <c r="L7" s="2">
+        <v>890</v>
+      </c>
+      <c r="M7" s="2">
+        <v>432</v>
+      </c>
+      <c r="N7" s="2">
+        <v>336</v>
+      </c>
+      <c r="O7" s="2">
+        <v>393</v>
+      </c>
+      <c r="P7" s="2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4806</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6597</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4451</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3371</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3037</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2264</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2319</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2226</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1586</v>
+      </c>
+      <c r="K8" s="2">
+        <v>628</v>
+      </c>
+      <c r="L8" s="2">
+        <v>893</v>
+      </c>
+      <c r="M8" s="2">
+        <v>359</v>
+      </c>
+      <c r="N8" s="2">
+        <v>234</v>
+      </c>
+      <c r="O8" s="2">
+        <v>402</v>
+      </c>
+      <c r="P8" s="2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4349</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4147</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3415</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4859</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2982</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1781</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1962</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1957</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1551</v>
+      </c>
+      <c r="K9" s="2">
+        <v>567</v>
+      </c>
+      <c r="L9" s="2">
+        <v>579</v>
+      </c>
+      <c r="M9" s="2">
+        <v>404</v>
+      </c>
+      <c r="N9" s="2">
+        <v>385</v>
+      </c>
+      <c r="O9" s="2">
+        <v>451</v>
+      </c>
+      <c r="P9" s="2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5244</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4083</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3252</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5230</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2805</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1976</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2022</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1639</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1662</v>
+      </c>
+      <c r="K10" s="2">
+        <v>556</v>
+      </c>
+      <c r="L10" s="2">
+        <v>595</v>
+      </c>
+      <c r="M10" s="2">
+        <v>352</v>
+      </c>
+      <c r="N10" s="2">
+        <v>369</v>
+      </c>
+      <c r="O10" s="2">
+        <v>425</v>
+      </c>
+      <c r="P10" s="2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4015</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3898</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2829</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6045</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3190</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2030</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1944</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1334</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1847</v>
+      </c>
+      <c r="K11" s="2">
+        <v>591</v>
+      </c>
+      <c r="L11" s="2">
+        <v>571</v>
+      </c>
+      <c r="M11" s="2">
+        <v>270</v>
+      </c>
+      <c r="N11" s="2">
+        <v>527</v>
+      </c>
+      <c r="O11" s="2">
+        <v>355</v>
+      </c>
+      <c r="P11" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3914</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3680</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2848</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5398</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3271</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2099</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1812</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1506</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2232</v>
+      </c>
+      <c r="K12" s="2">
+        <v>585</v>
+      </c>
+      <c r="L12" s="2">
+        <v>534</v>
+      </c>
+      <c r="M12" s="2">
+        <v>293</v>
+      </c>
+      <c r="N12" s="2">
+        <v>738</v>
+      </c>
+      <c r="O12" s="2">
+        <v>374</v>
+      </c>
+      <c r="P12" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4361</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4188</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2009</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4414</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3898</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2093</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2224</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1715</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2264</v>
+      </c>
+      <c r="K13" s="2">
+        <v>567</v>
+      </c>
+      <c r="L13" s="2">
+        <v>522</v>
+      </c>
+      <c r="M13" s="2">
+        <v>334</v>
+      </c>
+      <c r="N13" s="2">
+        <v>811</v>
+      </c>
+      <c r="O13" s="2">
+        <v>376</v>
+      </c>
+      <c r="P13" s="2">
+        <v>177</v>
+      </c>
+      <c r="Q13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>589</v>
-      </c>
-      <c r="C2">
-        <v>539</v>
-      </c>
-      <c r="D2">
-        <v>867</v>
-      </c>
-      <c r="E2">
-        <v>805</v>
-      </c>
-      <c r="F2">
-        <v>328</v>
-      </c>
-      <c r="G2">
-        <v>764</v>
-      </c>
-      <c r="H2">
-        <v>581</v>
-      </c>
-      <c r="J2">
-        <v>95</v>
-      </c>
-      <c r="K2">
-        <v>590</v>
-      </c>
-      <c r="L2">
-        <v>11</v>
-      </c>
-      <c r="M2">
-        <v>271</v>
-      </c>
-      <c r="N2">
-        <v>185</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
-      </c>
-      <c r="P2">
-        <v>144</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
-        <v>549</v>
-      </c>
-      <c r="C3">
-        <v>525</v>
-      </c>
-      <c r="D3">
-        <v>694</v>
-      </c>
-      <c r="E3">
-        <v>815</v>
-      </c>
-      <c r="F3">
-        <v>319</v>
-      </c>
-      <c r="G3">
-        <v>768</v>
-      </c>
-      <c r="H3">
-        <v>500</v>
-      </c>
-      <c r="J3">
-        <v>74</v>
-      </c>
-      <c r="K3">
-        <v>633</v>
-      </c>
-      <c r="L3">
-        <v>23</v>
-      </c>
-      <c r="M3">
-        <v>189</v>
-      </c>
-      <c r="N3">
-        <v>213</v>
-      </c>
-      <c r="O3">
-        <v>7</v>
-      </c>
-      <c r="P3">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>682</v>
-      </c>
-      <c r="C4">
-        <v>856</v>
-      </c>
-      <c r="D4">
-        <v>734</v>
-      </c>
-      <c r="E4">
-        <v>772</v>
-      </c>
-      <c r="F4">
-        <v>489</v>
-      </c>
-      <c r="G4">
-        <v>538</v>
-      </c>
-      <c r="H4">
-        <v>492</v>
-      </c>
-      <c r="I4">
-        <v>477</v>
-      </c>
-      <c r="J4">
-        <v>92</v>
-      </c>
-      <c r="K4">
-        <v>642</v>
-      </c>
-      <c r="L4">
-        <v>9</v>
-      </c>
-      <c r="M4">
-        <v>232</v>
-      </c>
-      <c r="N4">
-        <v>218</v>
-      </c>
-      <c r="O4">
-        <v>39</v>
-      </c>
-      <c r="P4">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>4434</v>
-      </c>
-      <c r="C5">
-        <v>3635</v>
-      </c>
-      <c r="D5">
-        <v>3799</v>
-      </c>
-      <c r="E5">
-        <v>1505</v>
-      </c>
-      <c r="F5">
-        <v>3464</v>
-      </c>
-      <c r="G5">
-        <v>2864</v>
-      </c>
-      <c r="H5">
-        <v>3344</v>
-      </c>
-      <c r="I5">
-        <v>2655</v>
-      </c>
-      <c r="J5">
-        <v>737</v>
-      </c>
-      <c r="K5">
-        <v>522</v>
-      </c>
-      <c r="L5">
-        <v>27</v>
-      </c>
-      <c r="M5">
-        <v>855</v>
-      </c>
-      <c r="N5">
-        <v>279</v>
-      </c>
-      <c r="O5">
-        <v>117</v>
-      </c>
-      <c r="P5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>14760</v>
-      </c>
-      <c r="C6">
-        <v>9280</v>
-      </c>
-      <c r="D6">
-        <v>11055</v>
-      </c>
-      <c r="E6">
-        <v>4296</v>
-      </c>
-      <c r="F6">
-        <v>5808</v>
-      </c>
-      <c r="G6">
-        <v>5380</v>
-      </c>
-      <c r="H6">
-        <v>4938</v>
-      </c>
-      <c r="I6">
-        <v>3645</v>
-      </c>
-      <c r="J6">
-        <v>4760</v>
-      </c>
-      <c r="K6">
-        <v>499</v>
-      </c>
-      <c r="L6">
-        <v>964</v>
-      </c>
-      <c r="M6">
-        <v>1145</v>
-      </c>
-      <c r="N6">
-        <v>323</v>
-      </c>
-      <c r="O6">
-        <v>291</v>
-      </c>
-      <c r="P6">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>10085</v>
-      </c>
-      <c r="C7">
-        <v>7736</v>
-      </c>
-      <c r="D7">
-        <v>6215</v>
-      </c>
-      <c r="E7">
-        <v>3788</v>
-      </c>
-      <c r="F7">
-        <v>3187</v>
-      </c>
-      <c r="G7">
-        <v>2914</v>
-      </c>
-      <c r="H7">
-        <v>2745</v>
-      </c>
-      <c r="I7">
-        <v>2865</v>
-      </c>
-      <c r="J7">
-        <v>2813</v>
-      </c>
-      <c r="K7">
-        <v>569</v>
-      </c>
-      <c r="L7">
-        <v>890</v>
-      </c>
-      <c r="M7">
-        <v>432</v>
-      </c>
-      <c r="N7">
-        <v>336</v>
-      </c>
-      <c r="O7">
-        <v>393</v>
-      </c>
-      <c r="P7">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>4806</v>
-      </c>
-      <c r="C8">
-        <v>6597</v>
-      </c>
-      <c r="D8">
-        <v>4451</v>
-      </c>
-      <c r="E8">
-        <v>3371</v>
-      </c>
-      <c r="F8">
-        <v>3037</v>
-      </c>
-      <c r="G8">
-        <v>2264</v>
-      </c>
-      <c r="H8">
-        <v>2319</v>
-      </c>
-      <c r="I8">
-        <v>2226</v>
-      </c>
-      <c r="J8">
-        <v>1586</v>
-      </c>
-      <c r="K8">
-        <v>628</v>
-      </c>
-      <c r="L8">
-        <v>893</v>
-      </c>
-      <c r="M8">
-        <v>359</v>
-      </c>
-      <c r="N8">
-        <v>234</v>
-      </c>
-      <c r="O8">
-        <v>402</v>
-      </c>
-      <c r="P8">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9">
-        <v>4349</v>
-      </c>
-      <c r="C9">
-        <v>4147</v>
-      </c>
-      <c r="D9">
-        <v>3415</v>
-      </c>
-      <c r="E9">
-        <v>4859</v>
-      </c>
-      <c r="F9">
-        <v>2982</v>
-      </c>
-      <c r="G9">
-        <v>1781</v>
-      </c>
-      <c r="H9">
-        <v>1962</v>
-      </c>
-      <c r="I9">
-        <v>1957</v>
-      </c>
-      <c r="J9">
-        <v>1551</v>
-      </c>
-      <c r="K9">
-        <v>567</v>
-      </c>
-      <c r="L9">
-        <v>579</v>
-      </c>
-      <c r="M9">
-        <v>404</v>
-      </c>
-      <c r="N9">
-        <v>385</v>
-      </c>
-      <c r="O9">
-        <v>451</v>
-      </c>
-      <c r="P9">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10">
-        <v>5244</v>
-      </c>
-      <c r="C10">
-        <v>4083</v>
-      </c>
-      <c r="D10">
-        <v>3252</v>
-      </c>
-      <c r="E10">
-        <v>5230</v>
-      </c>
-      <c r="F10">
-        <v>2805</v>
-      </c>
-      <c r="G10">
-        <v>1976</v>
-      </c>
-      <c r="H10">
-        <v>2022</v>
-      </c>
-      <c r="I10">
-        <v>1639</v>
-      </c>
-      <c r="J10">
-        <v>1662</v>
-      </c>
-      <c r="K10">
-        <v>556</v>
-      </c>
-      <c r="L10">
-        <v>595</v>
-      </c>
-      <c r="M10">
-        <v>352</v>
-      </c>
-      <c r="N10">
-        <v>369</v>
-      </c>
-      <c r="O10">
-        <v>425</v>
-      </c>
-      <c r="P10">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
-        <v>4015</v>
-      </c>
-      <c r="C11">
-        <v>3898</v>
-      </c>
-      <c r="D11">
-        <v>2829</v>
-      </c>
-      <c r="E11">
-        <v>6045</v>
-      </c>
-      <c r="F11">
-        <v>3190</v>
-      </c>
-      <c r="G11">
-        <v>2030</v>
-      </c>
-      <c r="H11">
-        <v>1944</v>
-      </c>
-      <c r="I11">
-        <v>1334</v>
-      </c>
-      <c r="J11">
-        <v>1847</v>
-      </c>
-      <c r="K11">
-        <v>591</v>
-      </c>
-      <c r="L11">
-        <v>571</v>
-      </c>
-      <c r="M11">
-        <v>270</v>
-      </c>
-      <c r="N11">
-        <v>527</v>
-      </c>
-      <c r="O11">
-        <v>355</v>
-      </c>
-      <c r="P11">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12">
-        <v>3914</v>
-      </c>
-      <c r="C12">
-        <v>3680</v>
-      </c>
-      <c r="D12">
-        <v>2848</v>
-      </c>
-      <c r="E12">
-        <v>5398</v>
-      </c>
-      <c r="F12">
-        <v>3271</v>
-      </c>
-      <c r="G12">
-        <v>2099</v>
-      </c>
-      <c r="H12">
-        <v>1812</v>
-      </c>
-      <c r="I12">
-        <v>1506</v>
-      </c>
-      <c r="J12">
-        <v>2232</v>
-      </c>
-      <c r="K12">
-        <v>585</v>
-      </c>
-      <c r="L12">
-        <v>534</v>
-      </c>
-      <c r="M12">
-        <v>293</v>
-      </c>
-      <c r="N12">
-        <v>738</v>
-      </c>
-      <c r="O12">
-        <v>374</v>
-      </c>
-      <c r="P12">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13">
-        <v>4361</v>
-      </c>
-      <c r="C13">
-        <v>4188</v>
-      </c>
-      <c r="D13">
-        <v>2009</v>
-      </c>
-      <c r="E13">
-        <v>4414</v>
-      </c>
-      <c r="F13">
-        <v>3898</v>
-      </c>
-      <c r="G13">
-        <v>2093</v>
-      </c>
-      <c r="H13">
-        <v>2224</v>
-      </c>
-      <c r="I13">
-        <v>1715</v>
-      </c>
-      <c r="J13">
-        <v>2264</v>
-      </c>
-      <c r="K13">
-        <v>567</v>
-      </c>
-      <c r="L13">
-        <v>522</v>
-      </c>
-      <c r="M13">
-        <v>334</v>
-      </c>
-      <c r="N13">
-        <v>811</v>
-      </c>
-      <c r="O13">
-        <v>376</v>
-      </c>
-      <c r="P13">
-        <v>177</v>
+      <c r="B14" s="6">
+        <f>SUM(B2:B13)</f>
+        <v>57788</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" ref="C14:P14" si="0">SUM(C2:C13)</f>
+        <v>49164</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>42168</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>41298</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>32778</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="0"/>
+        <v>25471</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>24883</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="0"/>
+        <v>20019</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="0"/>
+        <v>19713</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="0"/>
+        <v>6949</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="0"/>
+        <v>5618</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="0"/>
+        <v>5136</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="0"/>
+        <v>4618</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="0"/>
+        <v>3242</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="0"/>
+        <v>2835</v>
+      </c>
+      <c r="Q14" s="6">
+        <f>SUM(B14:P14)</f>
+        <v>341680</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>